<commit_message>
sampai diklat aja nih masih
</commit_message>
<xml_diff>
--- a/public/download_template/template_ASN_PNS.xlsx
+++ b/public/download_template/template_ASN_PNS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sikepeg\public\download_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Magang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC731DF-957D-4750-BD1D-5198AACB911C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{480969E8-0BEF-4D56-9DCE-6A4890884640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="15" windowWidth="26220" windowHeight="11505" xr2:uid="{79CF4374-6D94-4502-A1CB-04CCB44A2D7C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DE28BC7C-57A1-4DC0-A617-74539903B5D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>NIK</t>
   </si>
@@ -75,13 +84,22 @@
     <t>Status Tenaga</t>
   </si>
   <si>
+    <t>Status Tipe</t>
+  </si>
+  <si>
     <t>TMT CPNS</t>
   </si>
   <si>
     <t>TMT PNS</t>
   </si>
   <si>
-    <t>TMT Pangkat Terakhir</t>
+    <t>TMT Pangkat Akhir</t>
+  </si>
+  <si>
+    <t>Pangkat</t>
+  </si>
+  <si>
+    <t>Gol</t>
   </si>
   <si>
     <t>Pend Sesuai SK Terakhir</t>
@@ -102,56 +120,68 @@
     <t>Jabatan</t>
   </si>
   <si>
-    <t>Pangkat</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gol</t>
-  </si>
-  <si>
-    <t>Status Tipe</t>
-  </si>
-  <si>
-    <t>[struktural,umum,nakes]</t>
+    <t xml:space="preserve">Titis </t>
+  </si>
+  <si>
+    <t>Rahayu</t>
+  </si>
+  <si>
+    <t>S.M</t>
+  </si>
+  <si>
+    <t>[Perempuan, Laki-laki]</t>
+  </si>
+  <si>
+    <t>Banyuwangi</t>
+  </si>
+  <si>
+    <t>Jl. Brawijaya</t>
+  </si>
+  <si>
+    <t>Islam</t>
+  </si>
+  <si>
+    <t>082638110882</t>
+  </si>
+  <si>
+    <t>Aktif</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>PNS</t>
   </si>
   <si>
     <t>ASN</t>
   </si>
   <si>
-    <t>PNS</t>
-  </si>
-  <si>
-    <t>08</t>
-  </si>
-  <si>
-    <t>[AKTIF,NON AKTIF]</t>
-  </si>
-  <si>
-    <t>Titis</t>
-  </si>
-  <si>
-    <t>Esti</t>
-  </si>
-  <si>
-    <t>S.Tr</t>
-  </si>
-  <si>
-    <t>[laki-laki,perempuan]</t>
+    <t>Pembina</t>
+  </si>
+  <si>
+    <t>IV A</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>Universitas Jember</t>
+  </si>
+  <si>
+    <t>[struktural, nakes, umum]</t>
+  </si>
+  <si>
+    <t>Staff</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -165,7 +195,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -188,40 +218,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,47 +557,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7ACD44A-2474-4D61-BD3C-E4E255D98B09}">
-  <dimension ref="A1:AB4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D96EA83-5F0A-4A6D-8563-50A63F033D78}">
+  <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="8" customWidth="1"/>
-    <col min="10" max="10" width="16" style="5" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="5"/>
-    <col min="12" max="12" width="16.5703125" style="5" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="5" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" style="5" customWidth="1"/>
-    <col min="15" max="15" width="17" style="5" customWidth="1"/>
-    <col min="16" max="16" width="19.42578125" style="5" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" style="5" customWidth="1"/>
-    <col min="18" max="18" width="13.85546875" style="8" customWidth="1"/>
-    <col min="19" max="19" width="17.85546875" style="8" customWidth="1"/>
-    <col min="20" max="20" width="19.7109375" style="8" customWidth="1"/>
-    <col min="21" max="21" width="15.7109375" style="5" customWidth="1"/>
-    <col min="22" max="22" width="15.140625" style="5" customWidth="1"/>
-    <col min="23" max="23" width="21.28515625" style="5" customWidth="1"/>
-    <col min="24" max="24" width="25.140625" style="5" customWidth="1"/>
-    <col min="25" max="25" width="10.28515625" style="8" customWidth="1"/>
-    <col min="26" max="26" width="10" style="5" customWidth="1"/>
-    <col min="27" max="27" width="23.85546875" style="5" customWidth="1"/>
-    <col min="28" max="28" width="16.140625" style="5" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" style="5"/>
+    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21.77734375" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="12" width="12.77734375" customWidth="1"/>
+    <col min="13" max="13" width="16.5546875" customWidth="1"/>
+    <col min="14" max="14" width="20.21875" customWidth="1"/>
+    <col min="15" max="15" width="16.44140625" customWidth="1"/>
+    <col min="16" max="16" width="18.44140625" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" customWidth="1"/>
+    <col min="18" max="18" width="16.21875" style="6" customWidth="1"/>
+    <col min="19" max="19" width="19.77734375" style="6" customWidth="1"/>
+    <col min="20" max="20" width="16.88671875" style="6" customWidth="1"/>
+    <col min="21" max="21" width="13.33203125" customWidth="1"/>
+    <col min="23" max="23" width="23.44140625" customWidth="1"/>
+    <col min="24" max="24" width="22.21875" customWidth="1"/>
+    <col min="25" max="25" width="17.88671875" style="6" customWidth="1"/>
+    <col min="26" max="26" width="19.5546875" customWidth="1"/>
+    <col min="27" max="27" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -600,7 +617,7 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -621,107 +638,135 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>123</v>
+        <v>993</v>
       </c>
       <c r="B2" s="1">
-        <v>123</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10" t="s">
+        <v>3338</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="4">
+        <v>35983</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="K2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="L2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="6"/>
+      <c r="N2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="1">
+        <v>2040</v>
+      </c>
       <c r="P2" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="R2" s="4">
+        <v>47036</v>
+      </c>
+      <c r="S2" s="4">
+        <v>47027</v>
+      </c>
+      <c r="T2" s="4">
+        <v>46661</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y2" s="4">
+        <v>42287</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>3920</v>
+      </c>
       <c r="AA2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB2" s="1"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="L3" s="9"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="L4" s="9"/>
+        <v>44</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>